<commit_message>
t_l = -1% means ...
</commit_message>
<xml_diff>
--- a/Math results.xlsx
+++ b/Math results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\files\paper\My thesis\docker_volume\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E08C0D9-7719-47FC-804B-20EC912D7DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D880FD-71D2-40EC-8932-D0682B33B5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -974,12 +974,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1007,8 +1006,8 @@
       <xdr:rowOff>87923</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="214546" cy="281808"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="文字方塊 1">
@@ -1050,6 +1049,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1089,7 +1089,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="文字方塊 1">
@@ -1153,8 +1153,8 @@
       <xdr:rowOff>93784</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="400302" cy="281808"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="文字方塊 2">
@@ -1196,6 +1196,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1228,7 +1229,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="文字方塊 2">
@@ -1298,8 +1299,8 @@
       <xdr:rowOff>105507</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="167033" cy="281808"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="文字方塊 3">
@@ -1341,6 +1342,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1361,7 +1363,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="文字方塊 3">
@@ -1425,8 +1427,8 @@
       <xdr:rowOff>99645</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="478849" cy="281808"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="文字方塊 4">
@@ -1468,6 +1470,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1500,7 +1503,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="文字方塊 4">
@@ -1570,8 +1573,8 @@
       <xdr:rowOff>87922</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="614399" cy="299697"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="文字方塊 5">
@@ -1613,6 +1616,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1670,7 +1674,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="文字方塊 5">
@@ -1732,6 +1736,56 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>158262</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>99646</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2567354</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>637599</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="圖片 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{238F9CFA-3BB8-66B5-3F8F-D25F5F81E8F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4290647" y="99646"/>
+          <a:ext cx="2409092" cy="537953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2023,18 +2077,18 @@
   <dimension ref="A1:E241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="13.25" customWidth="1"/>
     <col min="5" max="5" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>